<commit_message>
Actualizar gráficas en Excel
</commit_message>
<xml_diff>
--- a/03_graficas/graficas_excel.xlsx
+++ b/03_graficas/graficas_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/segasi/Google Drive/R/04_medios/nexos/taller_de_datos/mios/tdd_victimas_homicidios/03_graficas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A02CB8-0ACE-744C-8986-98039A1D3AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BB189E-F635-BB42-8ECD-0779B1C2C09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3400" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{58F7AB5C-1D47-354D-9020-7039FEEB7FD7}"/>
   </bookViews>
@@ -116,6 +116,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX" sz="2000" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Réplica de la gráfica publicada por Alfonso Durazo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.6725650518622091E-2"/>
+          <c:y val="1.2195119609156979E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -162,6 +223,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.156663485544422E-2"/>
+                  <c:y val="-1.0309965371621784E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -175,16 +242,16 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
+                      <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     </a:defRPr>
                   </a:pPr>
                   <a:endParaRPr lang="es-MX"/>
@@ -595,8 +662,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.6495090920335983"/>
-                  <c:y val="0.13847798377607379"/>
+                  <c:x val="-0.71908475668329253"/>
+                  <c:y val="0.13766081473769642"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -612,16 +679,16 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
+                      <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     </a:defRPr>
                   </a:pPr>
                   <a:endParaRPr lang="es-MX"/>
@@ -890,16 +957,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-MX"/>
@@ -948,16 +1015,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-MX"/>
@@ -1006,7 +1073,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="es-MX"/>
     </a:p>
@@ -1033,6 +1103,92 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX" sz="2000" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Réplica de la gráfica publicada por David Pérez</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" sz="2000" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> Esparza</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX" sz="2000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.386785675605971E-2"/>
+          <c:y val="1.2807880779808326E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1063,7 +1219,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -1079,6 +1247,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5506847650013674E-2"/>
+                  <c:y val="-1.169416663220977E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1092,16 +1266,16 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
+                      <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     </a:defRPr>
                   </a:pPr>
                   <a:endParaRPr lang="es-MX"/>
@@ -1500,7 +1674,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -1518,8 +1704,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.43679770332890483"/>
-                  <c:y val="4.2579596201345077E-2"/>
+                  <c:x val="-0.54368106209294875"/>
+                  <c:y val="5.0492212311847071E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1535,16 +1721,16 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
+                      <a:cs typeface="Arial Narrow" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     </a:defRPr>
                   </a:pPr>
                   <a:endParaRPr lang="es-MX"/>
@@ -1786,6 +1972,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1535336351"/>
         <c:axId val="1543188431"/>
@@ -1844,6 +2031,7 @@
         <c:axId val="1543188431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3106,15 +3294,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>420076</xdr:colOff>
+      <xdr:colOff>420075</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>87922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>674076</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>166077</xdr:rowOff>
+      <xdr:colOff>722923</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3443,8 +3631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567DA282-A2AF-BE4B-9CCA-A88AF6794DA2}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3945,8 +4133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3251588F-1C81-434E-B0BB-FEDD498E7BF2}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>